<commit_message>
modified bulk promo script
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/OD/2023 PremiumVIP Promo - Product Import.xlsx
+++ b/src/test/java/testdata/OD/2023 PremiumVIP Promo - Product Import.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\github\OD_UI_Automation\src\test\java\testdata\OD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\github\core_UI_Automation\src\test\java\testdata\OD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282FD757-A5E9-48A3-997D-21215C9A8B89}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341EC23E-EE73-4424-90B7-7EF64F0EC3F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VIP Promos" sheetId="2" r:id="rId1"/>
     <sheet name="Staging" sheetId="3" r:id="rId2"/>
+    <sheet name="20 promos" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'VIP Promos'!$A$1:$AB$326</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6269" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6677" uniqueCount="366">
   <si>
     <t>Name</t>
   </si>
@@ -1530,8 +1531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CEE0A21-2F00-CE4A-80DF-F7E5013BA5D9}">
   <dimension ref="A1:AB326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O167" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24995,4 +24996,1569 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489367A9-E8D5-45F0-91B8-31D59E518767}">
+  <dimension ref="A1:AB21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>361</v>
+      </c>
+      <c r="L2">
+        <v>100</v>
+      </c>
+      <c r="M2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2">
+        <v>24</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" t="s">
+        <v>362</v>
+      </c>
+      <c r="U2" s="1"/>
+      <c r="V2" t="s">
+        <v>363</v>
+      </c>
+      <c r="X2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C3" t="s">
+        <v>359</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>361</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+      <c r="M3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3">
+        <v>24</v>
+      </c>
+      <c r="R3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" t="s">
+        <v>362</v>
+      </c>
+      <c r="U3" s="1"/>
+      <c r="V3" t="s">
+        <v>363</v>
+      </c>
+      <c r="X3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C4" t="s">
+        <v>359</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
+        <v>361</v>
+      </c>
+      <c r="L4">
+        <v>100</v>
+      </c>
+      <c r="M4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4">
+        <v>24</v>
+      </c>
+      <c r="R4" t="s">
+        <v>32</v>
+      </c>
+      <c r="S4" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" t="s">
+        <v>362</v>
+      </c>
+      <c r="U4" s="1"/>
+      <c r="V4" t="s">
+        <v>363</v>
+      </c>
+      <c r="X4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C5" t="s">
+        <v>359</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" t="s">
+        <v>361</v>
+      </c>
+      <c r="L5">
+        <v>100</v>
+      </c>
+      <c r="M5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5">
+        <v>24</v>
+      </c>
+      <c r="R5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T5" t="s">
+        <v>362</v>
+      </c>
+      <c r="U5" s="1"/>
+      <c r="V5" t="s">
+        <v>363</v>
+      </c>
+      <c r="X5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C6" t="s">
+        <v>359</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" t="s">
+        <v>361</v>
+      </c>
+      <c r="L6">
+        <v>100</v>
+      </c>
+      <c r="M6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="P6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q6">
+        <v>24</v>
+      </c>
+      <c r="R6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S6" t="s">
+        <v>32</v>
+      </c>
+      <c r="T6" t="s">
+        <v>362</v>
+      </c>
+      <c r="U6" s="1"/>
+      <c r="V6" t="s">
+        <v>363</v>
+      </c>
+      <c r="X6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C7" t="s">
+        <v>359</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" t="s">
+        <v>361</v>
+      </c>
+      <c r="L7">
+        <v>100</v>
+      </c>
+      <c r="M7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q7">
+        <v>24</v>
+      </c>
+      <c r="R7" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T7" t="s">
+        <v>362</v>
+      </c>
+      <c r="U7" s="1"/>
+      <c r="V7" t="s">
+        <v>363</v>
+      </c>
+      <c r="X7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C8" t="s">
+        <v>359</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
+        <v>361</v>
+      </c>
+      <c r="L8">
+        <v>100</v>
+      </c>
+      <c r="M8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" t="s">
+        <v>31</v>
+      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8">
+        <v>24</v>
+      </c>
+      <c r="R8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T8" t="s">
+        <v>362</v>
+      </c>
+      <c r="U8" s="1"/>
+      <c r="V8" t="s">
+        <v>363</v>
+      </c>
+      <c r="X8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C9" t="s">
+        <v>359</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" t="s">
+        <v>361</v>
+      </c>
+      <c r="L9">
+        <v>100</v>
+      </c>
+      <c r="M9" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" t="s">
+        <v>31</v>
+      </c>
+      <c r="O9" s="1"/>
+      <c r="P9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q9">
+        <v>24</v>
+      </c>
+      <c r="R9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S9" t="s">
+        <v>32</v>
+      </c>
+      <c r="T9" t="s">
+        <v>362</v>
+      </c>
+      <c r="U9" s="1"/>
+      <c r="V9" t="s">
+        <v>363</v>
+      </c>
+      <c r="X9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C10" t="s">
+        <v>359</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" t="s">
+        <v>361</v>
+      </c>
+      <c r="L10">
+        <v>100</v>
+      </c>
+      <c r="M10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" t="s">
+        <v>31</v>
+      </c>
+      <c r="O10" s="1"/>
+      <c r="P10" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q10">
+        <v>24</v>
+      </c>
+      <c r="R10" t="s">
+        <v>32</v>
+      </c>
+      <c r="S10" t="s">
+        <v>32</v>
+      </c>
+      <c r="T10" t="s">
+        <v>362</v>
+      </c>
+      <c r="U10" s="1"/>
+      <c r="V10" t="s">
+        <v>363</v>
+      </c>
+      <c r="X10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C11" t="s">
+        <v>359</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" t="s">
+        <v>361</v>
+      </c>
+      <c r="L11">
+        <v>100</v>
+      </c>
+      <c r="M11" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" t="s">
+        <v>31</v>
+      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q11">
+        <v>24</v>
+      </c>
+      <c r="R11" t="s">
+        <v>32</v>
+      </c>
+      <c r="S11" t="s">
+        <v>32</v>
+      </c>
+      <c r="T11" t="s">
+        <v>362</v>
+      </c>
+      <c r="U11" s="1"/>
+      <c r="V11" t="s">
+        <v>363</v>
+      </c>
+      <c r="X11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C12" t="s">
+        <v>359</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" t="s">
+        <v>361</v>
+      </c>
+      <c r="L12">
+        <v>100</v>
+      </c>
+      <c r="M12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" t="s">
+        <v>31</v>
+      </c>
+      <c r="O12" s="1"/>
+      <c r="P12" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12">
+        <v>24</v>
+      </c>
+      <c r="R12" t="s">
+        <v>32</v>
+      </c>
+      <c r="S12" t="s">
+        <v>32</v>
+      </c>
+      <c r="T12" t="s">
+        <v>362</v>
+      </c>
+      <c r="U12" s="1"/>
+      <c r="V12" t="s">
+        <v>363</v>
+      </c>
+      <c r="X12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C13" t="s">
+        <v>359</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" t="s">
+        <v>361</v>
+      </c>
+      <c r="L13">
+        <v>100</v>
+      </c>
+      <c r="M13" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" t="s">
+        <v>31</v>
+      </c>
+      <c r="O13" s="1"/>
+      <c r="P13" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q13">
+        <v>24</v>
+      </c>
+      <c r="R13" t="s">
+        <v>32</v>
+      </c>
+      <c r="S13" t="s">
+        <v>32</v>
+      </c>
+      <c r="T13" t="s">
+        <v>362</v>
+      </c>
+      <c r="U13" s="1"/>
+      <c r="V13" t="s">
+        <v>363</v>
+      </c>
+      <c r="X13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C14" t="s">
+        <v>359</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" t="s">
+        <v>361</v>
+      </c>
+      <c r="L14">
+        <v>100</v>
+      </c>
+      <c r="M14" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14" t="s">
+        <v>31</v>
+      </c>
+      <c r="O14" s="1"/>
+      <c r="P14" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q14">
+        <v>24</v>
+      </c>
+      <c r="R14" t="s">
+        <v>32</v>
+      </c>
+      <c r="S14" t="s">
+        <v>32</v>
+      </c>
+      <c r="T14" t="s">
+        <v>362</v>
+      </c>
+      <c r="U14" s="1"/>
+      <c r="V14" t="s">
+        <v>363</v>
+      </c>
+      <c r="X14" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C15" t="s">
+        <v>359</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" t="s">
+        <v>361</v>
+      </c>
+      <c r="L15">
+        <v>100</v>
+      </c>
+      <c r="M15" t="s">
+        <v>31</v>
+      </c>
+      <c r="N15" t="s">
+        <v>31</v>
+      </c>
+      <c r="O15" s="1"/>
+      <c r="P15" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q15">
+        <v>24</v>
+      </c>
+      <c r="R15" t="s">
+        <v>32</v>
+      </c>
+      <c r="S15" t="s">
+        <v>32</v>
+      </c>
+      <c r="T15" t="s">
+        <v>362</v>
+      </c>
+      <c r="U15" s="1"/>
+      <c r="V15" t="s">
+        <v>363</v>
+      </c>
+      <c r="X15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C16" t="s">
+        <v>359</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" t="s">
+        <v>361</v>
+      </c>
+      <c r="L16">
+        <v>100</v>
+      </c>
+      <c r="M16" t="s">
+        <v>31</v>
+      </c>
+      <c r="N16" t="s">
+        <v>31</v>
+      </c>
+      <c r="O16" s="1"/>
+      <c r="P16" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q16">
+        <v>24</v>
+      </c>
+      <c r="R16" t="s">
+        <v>32</v>
+      </c>
+      <c r="S16" t="s">
+        <v>32</v>
+      </c>
+      <c r="T16" t="s">
+        <v>362</v>
+      </c>
+      <c r="U16" s="1"/>
+      <c r="V16" t="s">
+        <v>363</v>
+      </c>
+      <c r="X16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C17" t="s">
+        <v>359</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K17" t="s">
+        <v>361</v>
+      </c>
+      <c r="L17">
+        <v>100</v>
+      </c>
+      <c r="M17" t="s">
+        <v>31</v>
+      </c>
+      <c r="N17" t="s">
+        <v>31</v>
+      </c>
+      <c r="O17" s="1"/>
+      <c r="P17" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q17">
+        <v>24</v>
+      </c>
+      <c r="R17" t="s">
+        <v>32</v>
+      </c>
+      <c r="S17" t="s">
+        <v>32</v>
+      </c>
+      <c r="T17" t="s">
+        <v>362</v>
+      </c>
+      <c r="U17" s="1"/>
+      <c r="V17" t="s">
+        <v>363</v>
+      </c>
+      <c r="X17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C18" t="s">
+        <v>359</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" t="s">
+        <v>361</v>
+      </c>
+      <c r="L18">
+        <v>100</v>
+      </c>
+      <c r="M18" t="s">
+        <v>31</v>
+      </c>
+      <c r="N18" t="s">
+        <v>31</v>
+      </c>
+      <c r="O18" s="1"/>
+      <c r="P18" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q18">
+        <v>24</v>
+      </c>
+      <c r="R18" t="s">
+        <v>32</v>
+      </c>
+      <c r="S18" t="s">
+        <v>32</v>
+      </c>
+      <c r="T18" t="s">
+        <v>362</v>
+      </c>
+      <c r="U18" s="1"/>
+      <c r="V18" t="s">
+        <v>363</v>
+      </c>
+      <c r="X18" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C19" t="s">
+        <v>359</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" t="s">
+        <v>361</v>
+      </c>
+      <c r="L19">
+        <v>100</v>
+      </c>
+      <c r="M19" t="s">
+        <v>31</v>
+      </c>
+      <c r="N19" t="s">
+        <v>31</v>
+      </c>
+      <c r="O19" s="1"/>
+      <c r="P19" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q19">
+        <v>24</v>
+      </c>
+      <c r="R19" t="s">
+        <v>32</v>
+      </c>
+      <c r="S19" t="s">
+        <v>32</v>
+      </c>
+      <c r="T19" t="s">
+        <v>362</v>
+      </c>
+      <c r="U19" s="1"/>
+      <c r="V19" t="s">
+        <v>363</v>
+      </c>
+      <c r="X19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C20" t="s">
+        <v>359</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" t="s">
+        <v>361</v>
+      </c>
+      <c r="L20">
+        <v>100</v>
+      </c>
+      <c r="M20" t="s">
+        <v>31</v>
+      </c>
+      <c r="N20" t="s">
+        <v>31</v>
+      </c>
+      <c r="O20" s="1"/>
+      <c r="P20" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q20">
+        <v>24</v>
+      </c>
+      <c r="R20" t="s">
+        <v>32</v>
+      </c>
+      <c r="S20" t="s">
+        <v>32</v>
+      </c>
+      <c r="T20" t="s">
+        <v>362</v>
+      </c>
+      <c r="U20" s="1"/>
+      <c r="V20" t="s">
+        <v>363</v>
+      </c>
+      <c r="X20" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C21" t="s">
+        <v>359</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K21" t="s">
+        <v>361</v>
+      </c>
+      <c r="L21">
+        <v>100</v>
+      </c>
+      <c r="M21" t="s">
+        <v>31</v>
+      </c>
+      <c r="N21" t="s">
+        <v>31</v>
+      </c>
+      <c r="O21" s="1"/>
+      <c r="P21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q21">
+        <v>24</v>
+      </c>
+      <c r="R21" t="s">
+        <v>32</v>
+      </c>
+      <c r="S21" t="s">
+        <v>32</v>
+      </c>
+      <c r="T21" t="s">
+        <v>362</v>
+      </c>
+      <c r="U21" s="1"/>
+      <c r="V21" t="s">
+        <v>363</v>
+      </c>
+      <c r="X21" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{AECE5662-3721-4D4F-B092-7D187E19EBCD}"/>
+    <hyperlink ref="B3:B21" r:id="rId2" display="sdumas@premiumparking.com" xr:uid="{EBCBC656-7663-452B-9E02-A152E230AE8E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated promo code script
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/OD/2023 PremiumVIP Promo - Product Import.xlsx
+++ b/src/test/java/testdata/OD/2023 PremiumVIP Promo - Product Import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\github\core_UI_Automation\src\test\java\testdata\OD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341EC23E-EE73-4424-90B7-7EF64F0EC3F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCC6BC9-E037-4A75-BC09-3B7AF3CE18E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VIP Promos" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="20 promos" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'VIP Promos'!$A$1:$AB$326</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'VIP Promos'!$A$1:$AB$288</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -1531,8 +1531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CEE0A21-2F00-CE4A-80DF-F7E5013BA5D9}">
   <dimension ref="A1:AB326"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>364</v>
@@ -1725,7 +1725,7 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>364</v>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>364</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>364</v>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>364</v>
@@ -2009,7 +2009,7 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>364</v>
@@ -2080,7 +2080,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>364</v>
@@ -2151,7 +2151,7 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>364</v>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>364</v>
@@ -2293,7 +2293,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>364</v>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>364</v>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>364</v>
@@ -2506,7 +2506,7 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>364</v>
@@ -2577,7 +2577,7 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>364</v>
@@ -2648,7 +2648,7 @@
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>364</v>
@@ -2719,7 +2719,7 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>364</v>
@@ -2790,7 +2790,7 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>364</v>
@@ -2861,7 +2861,7 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>364</v>
@@ -2932,7 +2932,7 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>364</v>
@@ -3003,7 +3003,7 @@
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>364</v>
@@ -3074,7 +3074,7 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>364</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>364</v>
@@ -3216,7 +3216,7 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>364</v>
@@ -3287,7 +3287,7 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>364</v>
@@ -3358,7 +3358,7 @@
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>364</v>
@@ -3429,7 +3429,7 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>364</v>
@@ -3500,7 +3500,7 @@
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>364</v>
@@ -3571,7 +3571,7 @@
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>364</v>
@@ -3642,7 +3642,7 @@
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>364</v>
@@ -3713,7 +3713,7 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>364</v>
@@ -3784,7 +3784,7 @@
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>364</v>
@@ -3855,7 +3855,7 @@
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>364</v>
@@ -3926,7 +3926,7 @@
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>364</v>
@@ -3997,7 +3997,7 @@
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>364</v>
@@ -4068,7 +4068,7 @@
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>364</v>
@@ -4139,7 +4139,7 @@
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>364</v>
@@ -4210,7 +4210,7 @@
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>364</v>
@@ -4281,7 +4281,7 @@
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>364</v>
@@ -4352,7 +4352,7 @@
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>364</v>
@@ -4423,7 +4423,7 @@
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>364</v>
@@ -4494,7 +4494,7 @@
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>364</v>
@@ -4565,7 +4565,7 @@
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>364</v>
@@ -4636,7 +4636,7 @@
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>364</v>
@@ -4707,7 +4707,7 @@
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>364</v>
@@ -4778,7 +4778,7 @@
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>364</v>
@@ -4808,7 +4808,7 @@
         <v>361</v>
       </c>
       <c r="L46">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M46" t="s">
         <v>31</v>
@@ -4849,7 +4849,7 @@
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>364</v>
@@ -4879,7 +4879,7 @@
         <v>361</v>
       </c>
       <c r="L47">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M47" t="s">
         <v>31</v>
@@ -4920,7 +4920,7 @@
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>364</v>
@@ -4950,7 +4950,7 @@
         <v>361</v>
       </c>
       <c r="L48">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M48" t="s">
         <v>31</v>
@@ -4991,7 +4991,7 @@
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>364</v>
@@ -5021,7 +5021,7 @@
         <v>361</v>
       </c>
       <c r="L49">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M49" t="s">
         <v>31</v>
@@ -5062,7 +5062,7 @@
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>364</v>
@@ -5092,7 +5092,7 @@
         <v>361</v>
       </c>
       <c r="L50">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M50" t="s">
         <v>31</v>
@@ -5133,7 +5133,7 @@
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>364</v>
@@ -5163,7 +5163,7 @@
         <v>361</v>
       </c>
       <c r="L51">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M51" t="s">
         <v>31</v>
@@ -5204,7 +5204,7 @@
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>364</v>
@@ -5234,7 +5234,7 @@
         <v>361</v>
       </c>
       <c r="L52">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M52" t="s">
         <v>31</v>
@@ -5275,7 +5275,7 @@
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>364</v>
@@ -5305,7 +5305,7 @@
         <v>361</v>
       </c>
       <c r="L53">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M53" t="s">
         <v>31</v>
@@ -5346,7 +5346,7 @@
     </row>
     <row r="54" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>364</v>
@@ -5376,7 +5376,7 @@
         <v>361</v>
       </c>
       <c r="L54">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M54" t="s">
         <v>31</v>
@@ -5417,7 +5417,7 @@
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>364</v>
@@ -5447,7 +5447,7 @@
         <v>361</v>
       </c>
       <c r="L55">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M55" t="s">
         <v>31</v>
@@ -5488,7 +5488,7 @@
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>364</v>
@@ -5518,7 +5518,7 @@
         <v>361</v>
       </c>
       <c r="L56">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M56" t="s">
         <v>31</v>
@@ -5559,7 +5559,7 @@
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>364</v>
@@ -5589,7 +5589,7 @@
         <v>361</v>
       </c>
       <c r="L57">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M57" t="s">
         <v>31</v>
@@ -5630,7 +5630,7 @@
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>364</v>
@@ -5660,7 +5660,7 @@
         <v>361</v>
       </c>
       <c r="L58">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M58" t="s">
         <v>31</v>
@@ -5701,7 +5701,7 @@
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>364</v>
@@ -5731,7 +5731,7 @@
         <v>361</v>
       </c>
       <c r="L59">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M59" t="s">
         <v>31</v>
@@ -5772,7 +5772,7 @@
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>364</v>
@@ -5802,7 +5802,7 @@
         <v>361</v>
       </c>
       <c r="L60">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M60" t="s">
         <v>31</v>
@@ -5843,7 +5843,7 @@
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>364</v>
@@ -5873,7 +5873,7 @@
         <v>361</v>
       </c>
       <c r="L61">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M61" t="s">
         <v>31</v>
@@ -5914,7 +5914,7 @@
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>364</v>
@@ -5944,7 +5944,7 @@
         <v>361</v>
       </c>
       <c r="L62">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="M62" t="s">
         <v>31</v>
@@ -5985,7 +5985,7 @@
     </row>
     <row r="63" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>364</v>
@@ -6015,7 +6015,7 @@
         <v>361</v>
       </c>
       <c r="L63">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M63" t="s">
         <v>31</v>
@@ -6056,7 +6056,7 @@
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>364</v>
@@ -6086,7 +6086,7 @@
         <v>361</v>
       </c>
       <c r="L64">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M64" t="s">
         <v>31</v>
@@ -6127,7 +6127,7 @@
     </row>
     <row r="65" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>364</v>
@@ -6157,7 +6157,7 @@
         <v>361</v>
       </c>
       <c r="L65">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M65" t="s">
         <v>31</v>
@@ -6198,7 +6198,7 @@
     </row>
     <row r="66" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>364</v>
@@ -6228,7 +6228,7 @@
         <v>361</v>
       </c>
       <c r="L66">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="M66" t="s">
         <v>31</v>
@@ -6269,7 +6269,7 @@
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>364</v>
@@ -6299,7 +6299,7 @@
         <v>361</v>
       </c>
       <c r="L67">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M67" t="s">
         <v>31</v>
@@ -6340,7 +6340,7 @@
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>364</v>
@@ -6370,7 +6370,7 @@
         <v>361</v>
       </c>
       <c r="L68">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M68" t="s">
         <v>31</v>
@@ -6411,7 +6411,7 @@
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>364</v>
@@ -6441,7 +6441,7 @@
         <v>361</v>
       </c>
       <c r="L69">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M69" t="s">
         <v>31</v>
@@ -6482,7 +6482,7 @@
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>364</v>
@@ -6512,7 +6512,7 @@
         <v>361</v>
       </c>
       <c r="L70">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="M70" t="s">
         <v>31</v>
@@ -6553,7 +6553,7 @@
     </row>
     <row r="71" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>364</v>
@@ -6583,7 +6583,7 @@
         <v>361</v>
       </c>
       <c r="L71">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M71" t="s">
         <v>31</v>
@@ -6624,7 +6624,7 @@
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>364</v>
@@ -6654,7 +6654,7 @@
         <v>361</v>
       </c>
       <c r="L72">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="M72" t="s">
         <v>31</v>
@@ -6695,7 +6695,7 @@
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>364</v>
@@ -6725,7 +6725,7 @@
         <v>361</v>
       </c>
       <c r="L73">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M73" t="s">
         <v>31</v>
@@ -6766,7 +6766,7 @@
     </row>
     <row r="74" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>106</v>
+        <v>144</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>364</v>
@@ -6796,7 +6796,7 @@
         <v>361</v>
       </c>
       <c r="L74">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M74" t="s">
         <v>31</v>
@@ -6837,7 +6837,7 @@
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>364</v>
@@ -6867,7 +6867,7 @@
         <v>361</v>
       </c>
       <c r="L75">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M75" t="s">
         <v>31</v>
@@ -6908,7 +6908,7 @@
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>364</v>
@@ -6938,7 +6938,7 @@
         <v>361</v>
       </c>
       <c r="L76">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M76" t="s">
         <v>31</v>
@@ -6979,7 +6979,7 @@
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>364</v>
@@ -7009,7 +7009,7 @@
         <v>361</v>
       </c>
       <c r="L77">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M77" t="s">
         <v>31</v>
@@ -7050,7 +7050,7 @@
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>110</v>
+        <v>148</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>364</v>
@@ -7080,7 +7080,7 @@
         <v>361</v>
       </c>
       <c r="L78">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M78" t="s">
         <v>31</v>
@@ -7121,7 +7121,7 @@
     </row>
     <row r="79" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>364</v>
@@ -7151,7 +7151,7 @@
         <v>361</v>
       </c>
       <c r="L79">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="M79" t="s">
         <v>31</v>
@@ -7192,7 +7192,7 @@
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>364</v>
@@ -7222,7 +7222,7 @@
         <v>361</v>
       </c>
       <c r="L80">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M80" t="s">
         <v>31</v>
@@ -7263,7 +7263,7 @@
     </row>
     <row r="81" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>364</v>
@@ -7293,7 +7293,7 @@
         <v>361</v>
       </c>
       <c r="L81">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M81" t="s">
         <v>31</v>
@@ -7334,7 +7334,7 @@
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>114</v>
+        <v>152</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>364</v>
@@ -7364,7 +7364,7 @@
         <v>361</v>
       </c>
       <c r="L82">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M82" t="s">
         <v>31</v>
@@ -7405,7 +7405,7 @@
     </row>
     <row r="83" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>364</v>
@@ -7435,7 +7435,7 @@
         <v>361</v>
       </c>
       <c r="L83">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M83" t="s">
         <v>31</v>
@@ -7476,7 +7476,7 @@
     </row>
     <row r="84" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>364</v>
@@ -7547,7 +7547,7 @@
     </row>
     <row r="85" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>117</v>
+        <v>155</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>364</v>
@@ -7577,7 +7577,7 @@
         <v>361</v>
       </c>
       <c r="L85">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="M85" t="s">
         <v>31</v>
@@ -7618,7 +7618,7 @@
     </row>
     <row r="86" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>118</v>
+        <v>156</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>364</v>
@@ -7689,7 +7689,7 @@
     </row>
     <row r="87" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>119</v>
+        <v>157</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>364</v>
@@ -7760,7 +7760,7 @@
     </row>
     <row r="88" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>364</v>
@@ -7831,7 +7831,7 @@
     </row>
     <row r="89" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>121</v>
+        <v>159</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>364</v>
@@ -7861,7 +7861,7 @@
         <v>361</v>
       </c>
       <c r="L89">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M89" t="s">
         <v>31</v>
@@ -7902,7 +7902,7 @@
     </row>
     <row r="90" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>122</v>
+        <v>160</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>364</v>
@@ -7973,7 +7973,7 @@
     </row>
     <row r="91" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>123</v>
+        <v>161</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>364</v>
@@ -8003,7 +8003,7 @@
         <v>361</v>
       </c>
       <c r="L91">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="M91" t="s">
         <v>31</v>
@@ -8044,7 +8044,7 @@
     </row>
     <row r="92" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>364</v>
@@ -8074,7 +8074,7 @@
         <v>361</v>
       </c>
       <c r="L92">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="M92" t="s">
         <v>31</v>
@@ -8115,7 +8115,7 @@
     </row>
     <row r="93" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>364</v>
@@ -8145,7 +8145,7 @@
         <v>361</v>
       </c>
       <c r="L93">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="M93" t="s">
         <v>31</v>
@@ -8186,7 +8186,7 @@
     </row>
     <row r="94" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>364</v>
@@ -8216,7 +8216,7 @@
         <v>361</v>
       </c>
       <c r="L94">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="M94" t="s">
         <v>31</v>
@@ -8257,7 +8257,7 @@
     </row>
     <row r="95" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>364</v>
@@ -8287,7 +8287,7 @@
         <v>361</v>
       </c>
       <c r="L95">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="M95" t="s">
         <v>31</v>
@@ -8328,7 +8328,7 @@
     </row>
     <row r="96" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>364</v>
@@ -8358,7 +8358,7 @@
         <v>361</v>
       </c>
       <c r="L96">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="M96" t="s">
         <v>31</v>
@@ -8399,7 +8399,7 @@
     </row>
     <row r="97" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>364</v>
@@ -8470,7 +8470,7 @@
     </row>
     <row r="98" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>364</v>
@@ -8541,7 +8541,7 @@
     </row>
     <row r="99" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>131</v>
+        <v>169</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>364</v>
@@ -8612,7 +8612,7 @@
     </row>
     <row r="100" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>364</v>
@@ -8642,7 +8642,7 @@
         <v>361</v>
       </c>
       <c r="L100">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="M100" t="s">
         <v>31</v>
@@ -8683,7 +8683,7 @@
     </row>
     <row r="101" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>364</v>
@@ -8713,7 +8713,7 @@
         <v>361</v>
       </c>
       <c r="L101">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="M101" t="s">
         <v>31</v>
@@ -8754,7 +8754,7 @@
     </row>
     <row r="102" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>134</v>
+        <v>172</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>364</v>
@@ -8784,7 +8784,7 @@
         <v>361</v>
       </c>
       <c r="L102">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="M102" t="s">
         <v>31</v>
@@ -8825,7 +8825,7 @@
     </row>
     <row r="103" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>135</v>
+        <v>173</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>364</v>
@@ -8896,7 +8896,7 @@
     </row>
     <row r="104" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>364</v>
@@ -8967,7 +8967,7 @@
     </row>
     <row r="105" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>364</v>
@@ -8997,7 +8997,7 @@
         <v>361</v>
       </c>
       <c r="L105">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="M105" t="s">
         <v>31</v>
@@ -9038,7 +9038,7 @@
     </row>
     <row r="106" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>138</v>
+        <v>176</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>364</v>
@@ -9068,7 +9068,7 @@
         <v>361</v>
       </c>
       <c r="L106">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="M106" t="s">
         <v>31</v>
@@ -9109,7 +9109,7 @@
     </row>
     <row r="107" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>364</v>
@@ -9139,7 +9139,7 @@
         <v>361</v>
       </c>
       <c r="L107">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="M107" t="s">
         <v>31</v>
@@ -9180,7 +9180,7 @@
     </row>
     <row r="108" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>140</v>
+        <v>178</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>364</v>
@@ -9210,7 +9210,7 @@
         <v>361</v>
       </c>
       <c r="L108">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="M108" t="s">
         <v>31</v>
@@ -9251,7 +9251,7 @@
     </row>
     <row r="109" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>141</v>
+        <v>179</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>364</v>
@@ -9281,7 +9281,7 @@
         <v>361</v>
       </c>
       <c r="L109">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="M109" t="s">
         <v>31</v>
@@ -9322,7 +9322,7 @@
     </row>
     <row r="110" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>142</v>
+        <v>180</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>364</v>
@@ -9352,7 +9352,7 @@
         <v>361</v>
       </c>
       <c r="L110">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="M110" t="s">
         <v>31</v>
@@ -9393,7 +9393,7 @@
     </row>
     <row r="111" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>143</v>
+        <v>181</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>364</v>
@@ -9423,7 +9423,7 @@
         <v>361</v>
       </c>
       <c r="L111">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="M111" t="s">
         <v>31</v>
@@ -9464,7 +9464,7 @@
     </row>
     <row r="112" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>144</v>
+        <v>182</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>364</v>
@@ -9535,7 +9535,7 @@
     </row>
     <row r="113" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>364</v>
@@ -9606,7 +9606,7 @@
     </row>
     <row r="114" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>146</v>
+        <v>184</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>364</v>
@@ -9636,7 +9636,7 @@
         <v>361</v>
       </c>
       <c r="L114">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="M114" t="s">
         <v>31</v>
@@ -9677,7 +9677,7 @@
     </row>
     <row r="115" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>364</v>
@@ -9748,7 +9748,7 @@
     </row>
     <row r="116" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>364</v>
@@ -9778,7 +9778,7 @@
         <v>361</v>
       </c>
       <c r="L116">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="M116" t="s">
         <v>31</v>
@@ -9819,7 +9819,7 @@
     </row>
     <row r="117" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>364</v>
@@ -9849,7 +9849,7 @@
         <v>361</v>
       </c>
       <c r="L117">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M117" t="s">
         <v>31</v>
@@ -9890,7 +9890,7 @@
     </row>
     <row r="118" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>364</v>
@@ -9920,7 +9920,7 @@
         <v>361</v>
       </c>
       <c r="L118">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="M118" t="s">
         <v>31</v>
@@ -9961,7 +9961,7 @@
     </row>
     <row r="119" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>364</v>
@@ -10032,7 +10032,7 @@
     </row>
     <row r="120" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>152</v>
+        <v>190</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>364</v>
@@ -10062,7 +10062,7 @@
         <v>361</v>
       </c>
       <c r="L120">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="M120" t="s">
         <v>31</v>
@@ -10103,7 +10103,7 @@
     </row>
     <row r="121" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>364</v>
@@ -10133,7 +10133,7 @@
         <v>361</v>
       </c>
       <c r="L121">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="M121" t="s">
         <v>31</v>
@@ -10174,7 +10174,7 @@
     </row>
     <row r="122" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>364</v>
@@ -10245,7 +10245,7 @@
     </row>
     <row r="123" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>155</v>
+        <v>193</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>364</v>
@@ -10275,7 +10275,7 @@
         <v>361</v>
       </c>
       <c r="L123">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="M123" t="s">
         <v>31</v>
@@ -10316,7 +10316,7 @@
     </row>
     <row r="124" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>156</v>
+        <v>194</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>364</v>
@@ -10387,7 +10387,7 @@
     </row>
     <row r="125" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>364</v>
@@ -10417,7 +10417,7 @@
         <v>361</v>
       </c>
       <c r="L125">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="M125" t="s">
         <v>31</v>
@@ -10458,7 +10458,7 @@
     </row>
     <row r="126" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>158</v>
+        <v>196</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>364</v>
@@ -10529,7 +10529,7 @@
     </row>
     <row r="127" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>159</v>
+        <v>197</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>364</v>
@@ -10559,7 +10559,7 @@
         <v>361</v>
       </c>
       <c r="L127">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M127" t="s">
         <v>31</v>
@@ -10600,7 +10600,7 @@
     </row>
     <row r="128" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>160</v>
+        <v>198</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>364</v>
@@ -10630,7 +10630,7 @@
         <v>361</v>
       </c>
       <c r="L128">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="M128" t="s">
         <v>31</v>
@@ -10671,7 +10671,7 @@
     </row>
     <row r="129" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>161</v>
+        <v>199</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>364</v>
@@ -10701,7 +10701,7 @@
         <v>361</v>
       </c>
       <c r="L129">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="M129" t="s">
         <v>31</v>
@@ -10742,7 +10742,7 @@
     </row>
     <row r="130" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>364</v>
@@ -10772,7 +10772,7 @@
         <v>361</v>
       </c>
       <c r="L130">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="M130" t="s">
         <v>31</v>
@@ -10813,7 +10813,7 @@
     </row>
     <row r="131" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>163</v>
+        <v>201</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>364</v>
@@ -10843,7 +10843,7 @@
         <v>361</v>
       </c>
       <c r="L131">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M131" t="s">
         <v>31</v>
@@ -10884,7 +10884,7 @@
     </row>
     <row r="132" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>164</v>
+        <v>202</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>364</v>
@@ -10914,7 +10914,7 @@
         <v>361</v>
       </c>
       <c r="L132">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M132" t="s">
         <v>31</v>
@@ -10955,7 +10955,7 @@
     </row>
     <row r="133" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>165</v>
+        <v>203</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>364</v>
@@ -11026,7 +11026,7 @@
     </row>
     <row r="134" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>166</v>
+        <v>204</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>364</v>
@@ -11056,7 +11056,7 @@
         <v>361</v>
       </c>
       <c r="L134">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M134" t="s">
         <v>31</v>
@@ -11097,7 +11097,7 @@
     </row>
     <row r="135" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>167</v>
+        <v>205</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>364</v>
@@ -11127,7 +11127,7 @@
         <v>361</v>
       </c>
       <c r="L135">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="M135" t="s">
         <v>31</v>
@@ -11168,7 +11168,7 @@
     </row>
     <row r="136" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>168</v>
+        <v>206</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>364</v>
@@ -11239,7 +11239,7 @@
     </row>
     <row r="137" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>169</v>
+        <v>207</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>364</v>
@@ -11269,7 +11269,7 @@
         <v>361</v>
       </c>
       <c r="L137">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="M137" t="s">
         <v>31</v>
@@ -11310,7 +11310,7 @@
     </row>
     <row r="138" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>170</v>
+        <v>208</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>364</v>
@@ -11340,7 +11340,7 @@
         <v>361</v>
       </c>
       <c r="L138">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="M138" t="s">
         <v>31</v>
@@ -11381,7 +11381,7 @@
     </row>
     <row r="139" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>171</v>
+        <v>209</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>364</v>
@@ -11452,7 +11452,7 @@
     </row>
     <row r="140" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>172</v>
+        <v>210</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>364</v>
@@ -11482,7 +11482,7 @@
         <v>361</v>
       </c>
       <c r="L140">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M140" t="s">
         <v>31</v>
@@ -11523,7 +11523,7 @@
     </row>
     <row r="141" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>173</v>
+        <v>211</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>364</v>
@@ -11594,7 +11594,7 @@
     </row>
     <row r="142" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>364</v>
@@ -11624,7 +11624,7 @@
         <v>361</v>
       </c>
       <c r="L142">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="M142" t="s">
         <v>31</v>
@@ -11665,7 +11665,7 @@
     </row>
     <row r="143" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>175</v>
+        <v>213</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>364</v>
@@ -11695,7 +11695,7 @@
         <v>361</v>
       </c>
       <c r="L143">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="M143" t="s">
         <v>31</v>
@@ -11736,7 +11736,7 @@
     </row>
     <row r="144" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>176</v>
+        <v>214</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>364</v>
@@ -11766,7 +11766,7 @@
         <v>361</v>
       </c>
       <c r="L144">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="M144" t="s">
         <v>31</v>
@@ -11807,7 +11807,7 @@
     </row>
     <row r="145" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>364</v>
@@ -11837,7 +11837,7 @@
         <v>361</v>
       </c>
       <c r="L145">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="M145" t="s">
         <v>31</v>
@@ -11878,7 +11878,7 @@
     </row>
     <row r="146" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>178</v>
+        <v>216</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>364</v>
@@ -11908,7 +11908,7 @@
         <v>361</v>
       </c>
       <c r="L146">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="M146" t="s">
         <v>31</v>
@@ -11949,7 +11949,7 @@
     </row>
     <row r="147" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>179</v>
+        <v>217</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>364</v>
@@ -11979,7 +11979,7 @@
         <v>361</v>
       </c>
       <c r="L147">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="M147" t="s">
         <v>31</v>
@@ -12020,7 +12020,7 @@
     </row>
     <row r="148" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>180</v>
+        <v>218</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>364</v>
@@ -12091,7 +12091,7 @@
     </row>
     <row r="149" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>181</v>
+        <v>219</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>364</v>
@@ -12121,7 +12121,7 @@
         <v>361</v>
       </c>
       <c r="L149">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M149" t="s">
         <v>31</v>
@@ -12162,7 +12162,7 @@
     </row>
     <row r="150" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>182</v>
+        <v>220</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>364</v>
@@ -12192,7 +12192,7 @@
         <v>361</v>
       </c>
       <c r="L150">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="M150" t="s">
         <v>31</v>
@@ -12233,7 +12233,7 @@
     </row>
     <row r="151" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>183</v>
+        <v>221</v>
       </c>
       <c r="B151" s="3" t="s">
         <v>364</v>
@@ -12263,7 +12263,7 @@
         <v>361</v>
       </c>
       <c r="L151">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="M151" t="s">
         <v>31</v>
@@ -12304,7 +12304,7 @@
     </row>
     <row r="152" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>184</v>
+        <v>222</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>364</v>
@@ -12334,7 +12334,7 @@
         <v>361</v>
       </c>
       <c r="L152">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M152" t="s">
         <v>31</v>
@@ -12375,7 +12375,7 @@
     </row>
     <row r="153" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>185</v>
+        <v>223</v>
       </c>
       <c r="B153" s="3" t="s">
         <v>364</v>
@@ -12446,7 +12446,7 @@
     </row>
     <row r="154" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>186</v>
+        <v>224</v>
       </c>
       <c r="B154" s="3" t="s">
         <v>364</v>
@@ -12476,7 +12476,7 @@
         <v>361</v>
       </c>
       <c r="L154">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="M154" t="s">
         <v>31</v>
@@ -12517,7 +12517,7 @@
     </row>
     <row r="155" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>187</v>
+        <v>225</v>
       </c>
       <c r="B155" s="3" t="s">
         <v>364</v>
@@ -12547,7 +12547,7 @@
         <v>361</v>
       </c>
       <c r="L155">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="M155" t="s">
         <v>31</v>
@@ -12588,7 +12588,7 @@
     </row>
     <row r="156" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>188</v>
+        <v>226</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>364</v>
@@ -12618,7 +12618,7 @@
         <v>361</v>
       </c>
       <c r="L156">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M156" t="s">
         <v>31</v>
@@ -12659,7 +12659,7 @@
     </row>
     <row r="157" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>189</v>
+        <v>227</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>364</v>
@@ -12689,7 +12689,7 @@
         <v>361</v>
       </c>
       <c r="L157">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M157" t="s">
         <v>31</v>
@@ -12730,7 +12730,7 @@
     </row>
     <row r="158" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>190</v>
+        <v>228</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>364</v>
@@ -12760,7 +12760,7 @@
         <v>361</v>
       </c>
       <c r="L158">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M158" t="s">
         <v>31</v>
@@ -12801,7 +12801,7 @@
     </row>
     <row r="159" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>191</v>
+        <v>229</v>
       </c>
       <c r="B159" s="3" t="s">
         <v>364</v>
@@ -12831,7 +12831,7 @@
         <v>361</v>
       </c>
       <c r="L159">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M159" t="s">
         <v>31</v>
@@ -12872,7 +12872,7 @@
     </row>
     <row r="160" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>192</v>
+        <v>230</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>364</v>
@@ -12902,7 +12902,7 @@
         <v>361</v>
       </c>
       <c r="L160">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M160" t="s">
         <v>31</v>
@@ -12943,7 +12943,7 @@
     </row>
     <row r="161" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>193</v>
+        <v>231</v>
       </c>
       <c r="B161" s="3" t="s">
         <v>364</v>
@@ -12973,7 +12973,7 @@
         <v>361</v>
       </c>
       <c r="L161">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M161" t="s">
         <v>31</v>
@@ -13014,7 +13014,7 @@
     </row>
     <row r="162" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>194</v>
+        <v>232</v>
       </c>
       <c r="B162" s="3" t="s">
         <v>364</v>
@@ -13044,7 +13044,7 @@
         <v>361</v>
       </c>
       <c r="L162">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M162" t="s">
         <v>31</v>
@@ -13085,7 +13085,7 @@
     </row>
     <row r="163" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>195</v>
+        <v>233</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>364</v>
@@ -13115,7 +13115,7 @@
         <v>361</v>
       </c>
       <c r="L163">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M163" t="s">
         <v>31</v>
@@ -13156,7 +13156,7 @@
     </row>
     <row r="164" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>196</v>
+        <v>234</v>
       </c>
       <c r="B164" s="3" t="s">
         <v>364</v>
@@ -13186,7 +13186,7 @@
         <v>361</v>
       </c>
       <c r="L164">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M164" t="s">
         <v>31</v>
@@ -13227,7 +13227,7 @@
     </row>
     <row r="165" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>197</v>
+        <v>235</v>
       </c>
       <c r="B165" s="3" t="s">
         <v>364</v>
@@ -13257,7 +13257,7 @@
         <v>361</v>
       </c>
       <c r="L165">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M165" t="s">
         <v>31</v>
@@ -13298,7 +13298,7 @@
     </row>
     <row r="166" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>198</v>
+        <v>236</v>
       </c>
       <c r="B166" s="3" t="s">
         <v>364</v>
@@ -13328,7 +13328,7 @@
         <v>361</v>
       </c>
       <c r="L166">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M166" t="s">
         <v>31</v>
@@ -13369,7 +13369,7 @@
     </row>
     <row r="167" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>199</v>
+        <v>237</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>364</v>
@@ -13399,7 +13399,7 @@
         <v>361</v>
       </c>
       <c r="L167">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M167" t="s">
         <v>31</v>
@@ -13440,7 +13440,7 @@
     </row>
     <row r="168" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>200</v>
+        <v>238</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>364</v>
@@ -13470,7 +13470,7 @@
         <v>361</v>
       </c>
       <c r="L168">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M168" t="s">
         <v>31</v>
@@ -13511,7 +13511,7 @@
     </row>
     <row r="169" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>201</v>
+        <v>239</v>
       </c>
       <c r="B169" s="3" t="s">
         <v>364</v>
@@ -13541,7 +13541,7 @@
         <v>361</v>
       </c>
       <c r="L169">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="M169" t="s">
         <v>31</v>
@@ -13582,7 +13582,7 @@
     </row>
     <row r="170" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>202</v>
+        <v>240</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>364</v>
@@ -13612,7 +13612,7 @@
         <v>361</v>
       </c>
       <c r="L170">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M170" t="s">
         <v>31</v>
@@ -13653,7 +13653,7 @@
     </row>
     <row r="171" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>203</v>
+        <v>241</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>364</v>
@@ -13683,7 +13683,7 @@
         <v>361</v>
       </c>
       <c r="L171">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M171" t="s">
         <v>31</v>
@@ -13724,7 +13724,7 @@
     </row>
     <row r="172" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>204</v>
+        <v>242</v>
       </c>
       <c r="B172" s="3" t="s">
         <v>364</v>
@@ -13754,7 +13754,7 @@
         <v>361</v>
       </c>
       <c r="L172">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="M172" t="s">
         <v>31</v>
@@ -13795,7 +13795,7 @@
     </row>
     <row r="173" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>205</v>
+        <v>243</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>364</v>
@@ -13825,7 +13825,7 @@
         <v>361</v>
       </c>
       <c r="L173">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M173" t="s">
         <v>31</v>
@@ -13866,7 +13866,7 @@
     </row>
     <row r="174" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>206</v>
+        <v>244</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>364</v>
@@ -13896,7 +13896,7 @@
         <v>361</v>
       </c>
       <c r="L174">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M174" t="s">
         <v>31</v>
@@ -13937,7 +13937,7 @@
     </row>
     <row r="175" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>207</v>
+        <v>245</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>364</v>
@@ -13967,7 +13967,7 @@
         <v>361</v>
       </c>
       <c r="L175">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M175" t="s">
         <v>31</v>
@@ -14008,7 +14008,7 @@
     </row>
     <row r="176" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>208</v>
+        <v>246</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>364</v>
@@ -14038,7 +14038,7 @@
         <v>361</v>
       </c>
       <c r="L176">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M176" t="s">
         <v>31</v>
@@ -14079,7 +14079,7 @@
     </row>
     <row r="177" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>209</v>
+        <v>247</v>
       </c>
       <c r="B177" s="3" t="s">
         <v>364</v>
@@ -14109,7 +14109,7 @@
         <v>361</v>
       </c>
       <c r="L177">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M177" t="s">
         <v>31</v>
@@ -14150,7 +14150,7 @@
     </row>
     <row r="178" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>210</v>
+        <v>248</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>364</v>
@@ -14180,7 +14180,7 @@
         <v>361</v>
       </c>
       <c r="L178">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M178" t="s">
         <v>31</v>
@@ -14221,7 +14221,7 @@
     </row>
     <row r="179" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>211</v>
+        <v>249</v>
       </c>
       <c r="B179" s="3" t="s">
         <v>364</v>
@@ -14251,7 +14251,7 @@
         <v>361</v>
       </c>
       <c r="L179">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M179" t="s">
         <v>31</v>
@@ -14292,7 +14292,7 @@
     </row>
     <row r="180" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>212</v>
+        <v>250</v>
       </c>
       <c r="B180" s="3" t="s">
         <v>364</v>
@@ -14322,7 +14322,7 @@
         <v>361</v>
       </c>
       <c r="L180">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M180" t="s">
         <v>31</v>
@@ -14363,7 +14363,7 @@
     </row>
     <row r="181" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>213</v>
+        <v>251</v>
       </c>
       <c r="B181" s="3" t="s">
         <v>364</v>
@@ -14393,7 +14393,7 @@
         <v>361</v>
       </c>
       <c r="L181">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="M181" t="s">
         <v>31</v>
@@ -14434,7 +14434,7 @@
     </row>
     <row r="182" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>214</v>
+        <v>252</v>
       </c>
       <c r="B182" s="3" t="s">
         <v>364</v>
@@ -14464,7 +14464,7 @@
         <v>361</v>
       </c>
       <c r="L182">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="M182" t="s">
         <v>31</v>
@@ -14505,7 +14505,7 @@
     </row>
     <row r="183" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>215</v>
+        <v>253</v>
       </c>
       <c r="B183" s="3" t="s">
         <v>364</v>
@@ -14535,7 +14535,7 @@
         <v>361</v>
       </c>
       <c r="L183">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M183" t="s">
         <v>31</v>
@@ -14576,7 +14576,7 @@
     </row>
     <row r="184" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>216</v>
+        <v>254</v>
       </c>
       <c r="B184" s="3" t="s">
         <v>364</v>
@@ -14606,7 +14606,7 @@
         <v>361</v>
       </c>
       <c r="L184">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M184" t="s">
         <v>31</v>
@@ -14647,7 +14647,7 @@
     </row>
     <row r="185" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>217</v>
+        <v>255</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>364</v>
@@ -14677,7 +14677,7 @@
         <v>361</v>
       </c>
       <c r="L185">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M185" t="s">
         <v>31</v>
@@ -14718,7 +14718,7 @@
     </row>
     <row r="186" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>218</v>
+        <v>256</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>364</v>
@@ -14748,7 +14748,7 @@
         <v>361</v>
       </c>
       <c r="L186">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M186" t="s">
         <v>31</v>
@@ -14789,7 +14789,7 @@
     </row>
     <row r="187" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>219</v>
+        <v>257</v>
       </c>
       <c r="B187" s="3" t="s">
         <v>364</v>
@@ -14819,7 +14819,7 @@
         <v>361</v>
       </c>
       <c r="L187">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M187" t="s">
         <v>31</v>
@@ -14860,7 +14860,7 @@
     </row>
     <row r="188" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>220</v>
+        <v>258</v>
       </c>
       <c r="B188" s="3" t="s">
         <v>364</v>
@@ -14890,7 +14890,7 @@
         <v>361</v>
       </c>
       <c r="L188">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M188" t="s">
         <v>31</v>
@@ -14931,7 +14931,7 @@
     </row>
     <row r="189" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>221</v>
+        <v>259</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>364</v>
@@ -14961,7 +14961,7 @@
         <v>361</v>
       </c>
       <c r="L189">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M189" t="s">
         <v>31</v>
@@ -15002,7 +15002,7 @@
     </row>
     <row r="190" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>222</v>
+        <v>260</v>
       </c>
       <c r="B190" s="3" t="s">
         <v>364</v>
@@ -15032,7 +15032,7 @@
         <v>361</v>
       </c>
       <c r="L190">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M190" t="s">
         <v>31</v>
@@ -15073,7 +15073,7 @@
     </row>
     <row r="191" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>223</v>
+        <v>261</v>
       </c>
       <c r="B191" s="3" t="s">
         <v>364</v>
@@ -15103,7 +15103,7 @@
         <v>361</v>
       </c>
       <c r="L191">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="M191" t="s">
         <v>31</v>
@@ -15144,7 +15144,7 @@
     </row>
     <row r="192" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>224</v>
+        <v>262</v>
       </c>
       <c r="B192" s="3" t="s">
         <v>364</v>
@@ -15174,7 +15174,7 @@
         <v>361</v>
       </c>
       <c r="L192">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M192" t="s">
         <v>31</v>
@@ -15215,7 +15215,7 @@
     </row>
     <row r="193" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>225</v>
+        <v>263</v>
       </c>
       <c r="B193" s="3" t="s">
         <v>364</v>
@@ -15286,7 +15286,7 @@
     </row>
     <row r="194" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>226</v>
+        <v>264</v>
       </c>
       <c r="B194" s="3" t="s">
         <v>364</v>
@@ -15316,7 +15316,7 @@
         <v>361</v>
       </c>
       <c r="L194">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M194" t="s">
         <v>31</v>
@@ -15357,7 +15357,7 @@
     </row>
     <row r="195" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>227</v>
+        <v>265</v>
       </c>
       <c r="B195" s="3" t="s">
         <v>364</v>
@@ -15428,7 +15428,7 @@
     </row>
     <row r="196" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>228</v>
+        <v>266</v>
       </c>
       <c r="B196" s="3" t="s">
         <v>364</v>
@@ -15499,7 +15499,7 @@
     </row>
     <row r="197" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>229</v>
+        <v>267</v>
       </c>
       <c r="B197" s="3" t="s">
         <v>364</v>
@@ -15570,7 +15570,7 @@
     </row>
     <row r="198" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>230</v>
+        <v>268</v>
       </c>
       <c r="B198" s="3" t="s">
         <v>364</v>
@@ -15641,7 +15641,7 @@
     </row>
     <row r="199" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>231</v>
+        <v>269</v>
       </c>
       <c r="B199" s="3" t="s">
         <v>364</v>
@@ -15712,7 +15712,7 @@
     </row>
     <row r="200" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>232</v>
+        <v>270</v>
       </c>
       <c r="B200" s="3" t="s">
         <v>364</v>
@@ -15783,7 +15783,7 @@
     </row>
     <row r="201" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>233</v>
+        <v>271</v>
       </c>
       <c r="B201" s="3" t="s">
         <v>364</v>
@@ -15854,7 +15854,7 @@
     </row>
     <row r="202" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>234</v>
+        <v>272</v>
       </c>
       <c r="B202" s="3" t="s">
         <v>364</v>
@@ -15925,7 +15925,7 @@
     </row>
     <row r="203" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="B203" s="3" t="s">
         <v>364</v>
@@ -15996,7 +15996,7 @@
     </row>
     <row r="204" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>236</v>
+        <v>274</v>
       </c>
       <c r="B204" s="3" t="s">
         <v>364</v>
@@ -16067,7 +16067,7 @@
     </row>
     <row r="205" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>237</v>
+        <v>275</v>
       </c>
       <c r="B205" s="3" t="s">
         <v>364</v>
@@ -16138,7 +16138,7 @@
     </row>
     <row r="206" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>238</v>
+        <v>276</v>
       </c>
       <c r="B206" s="3" t="s">
         <v>364</v>
@@ -16209,7 +16209,7 @@
     </row>
     <row r="207" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>239</v>
+        <v>277</v>
       </c>
       <c r="B207" s="3" t="s">
         <v>364</v>
@@ -16239,7 +16239,7 @@
         <v>361</v>
       </c>
       <c r="L207">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M207" t="s">
         <v>31</v>
@@ -16280,7 +16280,7 @@
     </row>
     <row r="208" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>240</v>
+        <v>278</v>
       </c>
       <c r="B208" s="3" t="s">
         <v>364</v>
@@ -16351,7 +16351,7 @@
     </row>
     <row r="209" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>241</v>
+        <v>279</v>
       </c>
       <c r="B209" s="3" t="s">
         <v>364</v>
@@ -16422,7 +16422,7 @@
     </row>
     <row r="210" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>242</v>
+        <v>280</v>
       </c>
       <c r="B210" s="3" t="s">
         <v>364</v>
@@ -16493,7 +16493,7 @@
     </row>
     <row r="211" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>243</v>
+        <v>281</v>
       </c>
       <c r="B211" s="3" t="s">
         <v>364</v>
@@ -16564,7 +16564,7 @@
     </row>
     <row r="212" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>244</v>
+        <v>282</v>
       </c>
       <c r="B212" s="3" t="s">
         <v>364</v>
@@ -16635,7 +16635,7 @@
     </row>
     <row r="213" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>245</v>
+        <v>283</v>
       </c>
       <c r="B213" s="3" t="s">
         <v>364</v>
@@ -16706,7 +16706,7 @@
     </row>
     <row r="214" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>246</v>
+        <v>284</v>
       </c>
       <c r="B214" s="3" t="s">
         <v>364</v>
@@ -16777,7 +16777,7 @@
     </row>
     <row r="215" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>247</v>
+        <v>285</v>
       </c>
       <c r="B215" s="3" t="s">
         <v>364</v>
@@ -16848,7 +16848,7 @@
     </row>
     <row r="216" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>248</v>
+        <v>286</v>
       </c>
       <c r="B216" s="3" t="s">
         <v>364</v>
@@ -16919,7 +16919,7 @@
     </row>
     <row r="217" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>249</v>
+        <v>287</v>
       </c>
       <c r="B217" s="3" t="s">
         <v>364</v>
@@ -16990,7 +16990,7 @@
     </row>
     <row r="218" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>250</v>
+        <v>288</v>
       </c>
       <c r="B218" s="3" t="s">
         <v>364</v>
@@ -17061,7 +17061,7 @@
     </row>
     <row r="219" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>251</v>
+        <v>289</v>
       </c>
       <c r="B219" s="3" t="s">
         <v>364</v>
@@ -17132,7 +17132,7 @@
     </row>
     <row r="220" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>252</v>
+        <v>290</v>
       </c>
       <c r="B220" s="3" t="s">
         <v>364</v>
@@ -17203,7 +17203,7 @@
     </row>
     <row r="221" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>253</v>
+        <v>291</v>
       </c>
       <c r="B221" s="3" t="s">
         <v>364</v>
@@ -17274,7 +17274,7 @@
     </row>
     <row r="222" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>254</v>
+        <v>292</v>
       </c>
       <c r="B222" s="3" t="s">
         <v>364</v>
@@ -17345,7 +17345,7 @@
     </row>
     <row r="223" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>255</v>
+        <v>293</v>
       </c>
       <c r="B223" s="3" t="s">
         <v>364</v>
@@ -17416,7 +17416,7 @@
     </row>
     <row r="224" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>256</v>
+        <v>294</v>
       </c>
       <c r="B224" s="3" t="s">
         <v>364</v>
@@ -17487,7 +17487,7 @@
     </row>
     <row r="225" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>257</v>
+        <v>295</v>
       </c>
       <c r="B225" s="3" t="s">
         <v>364</v>
@@ -17558,7 +17558,7 @@
     </row>
     <row r="226" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>258</v>
+        <v>296</v>
       </c>
       <c r="B226" s="3" t="s">
         <v>364</v>
@@ -17629,7 +17629,7 @@
     </row>
     <row r="227" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>259</v>
+        <v>297</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>364</v>
@@ -17700,7 +17700,7 @@
     </row>
     <row r="228" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>260</v>
+        <v>298</v>
       </c>
       <c r="B228" s="3" t="s">
         <v>364</v>
@@ -17771,7 +17771,7 @@
     </row>
     <row r="229" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>261</v>
+        <v>299</v>
       </c>
       <c r="B229" s="3" t="s">
         <v>364</v>
@@ -17842,7 +17842,7 @@
     </row>
     <row r="230" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>262</v>
+        <v>300</v>
       </c>
       <c r="B230" s="3" t="s">
         <v>364</v>
@@ -17913,7 +17913,7 @@
     </row>
     <row r="231" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>263</v>
+        <v>301</v>
       </c>
       <c r="B231" s="3" t="s">
         <v>364</v>
@@ -17943,7 +17943,7 @@
         <v>361</v>
       </c>
       <c r="L231">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M231" t="s">
         <v>31</v>
@@ -17984,7 +17984,7 @@
     </row>
     <row r="232" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>264</v>
+        <v>302</v>
       </c>
       <c r="B232" s="3" t="s">
         <v>364</v>
@@ -18014,7 +18014,7 @@
         <v>361</v>
       </c>
       <c r="L232">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M232" t="s">
         <v>31</v>
@@ -18055,7 +18055,7 @@
     </row>
     <row r="233" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>265</v>
+        <v>303</v>
       </c>
       <c r="B233" s="3" t="s">
         <v>364</v>
@@ -18126,7 +18126,7 @@
     </row>
     <row r="234" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>266</v>
+        <v>304</v>
       </c>
       <c r="B234" s="3" t="s">
         <v>364</v>
@@ -18197,7 +18197,7 @@
     </row>
     <row r="235" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>267</v>
+        <v>305</v>
       </c>
       <c r="B235" s="3" t="s">
         <v>364</v>
@@ -18268,7 +18268,7 @@
     </row>
     <row r="236" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>268</v>
+        <v>306</v>
       </c>
       <c r="B236" s="3" t="s">
         <v>364</v>
@@ -18339,7 +18339,7 @@
     </row>
     <row r="237" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>269</v>
+        <v>307</v>
       </c>
       <c r="B237" s="3" t="s">
         <v>364</v>
@@ -18410,7 +18410,7 @@
     </row>
     <row r="238" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>270</v>
+        <v>308</v>
       </c>
       <c r="B238" s="3" t="s">
         <v>364</v>
@@ -18481,7 +18481,7 @@
     </row>
     <row r="239" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>271</v>
+        <v>309</v>
       </c>
       <c r="B239" s="3" t="s">
         <v>364</v>
@@ -18552,7 +18552,7 @@
     </row>
     <row r="240" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>272</v>
+        <v>310</v>
       </c>
       <c r="B240" s="3" t="s">
         <v>364</v>
@@ -18623,7 +18623,7 @@
     </row>
     <row r="241" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>273</v>
+        <v>311</v>
       </c>
       <c r="B241" s="3" t="s">
         <v>364</v>
@@ -18694,7 +18694,7 @@
     </row>
     <row r="242" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>274</v>
+        <v>312</v>
       </c>
       <c r="B242" s="3" t="s">
         <v>364</v>
@@ -18765,7 +18765,7 @@
     </row>
     <row r="243" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>275</v>
+        <v>313</v>
       </c>
       <c r="B243" s="3" t="s">
         <v>364</v>
@@ -18836,7 +18836,7 @@
     </row>
     <row r="244" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>276</v>
+        <v>314</v>
       </c>
       <c r="B244" s="3" t="s">
         <v>364</v>
@@ -18907,7 +18907,7 @@
     </row>
     <row r="245" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>277</v>
+        <v>315</v>
       </c>
       <c r="B245" s="3" t="s">
         <v>364</v>
@@ -18978,7 +18978,7 @@
     </row>
     <row r="246" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>278</v>
+        <v>316</v>
       </c>
       <c r="B246" s="3" t="s">
         <v>364</v>
@@ -19049,7 +19049,7 @@
     </row>
     <row r="247" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>279</v>
+        <v>317</v>
       </c>
       <c r="B247" s="3" t="s">
         <v>364</v>
@@ -19120,7 +19120,7 @@
     </row>
     <row r="248" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>280</v>
+        <v>318</v>
       </c>
       <c r="B248" s="3" t="s">
         <v>364</v>
@@ -19191,7 +19191,7 @@
     </row>
     <row r="249" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>281</v>
+        <v>319</v>
       </c>
       <c r="B249" s="3" t="s">
         <v>364</v>
@@ -19262,7 +19262,7 @@
     </row>
     <row r="250" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>282</v>
+        <v>320</v>
       </c>
       <c r="B250" s="3" t="s">
         <v>364</v>
@@ -19333,7 +19333,7 @@
     </row>
     <row r="251" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>283</v>
+        <v>321</v>
       </c>
       <c r="B251" s="3" t="s">
         <v>364</v>
@@ -19404,7 +19404,7 @@
     </row>
     <row r="252" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>284</v>
+        <v>322</v>
       </c>
       <c r="B252" s="3" t="s">
         <v>364</v>
@@ -19475,7 +19475,7 @@
     </row>
     <row r="253" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>285</v>
+        <v>323</v>
       </c>
       <c r="B253" s="3" t="s">
         <v>364</v>
@@ -19546,7 +19546,7 @@
     </row>
     <row r="254" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>286</v>
+        <v>324</v>
       </c>
       <c r="B254" s="3" t="s">
         <v>364</v>
@@ -19617,7 +19617,7 @@
     </row>
     <row r="255" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>287</v>
+        <v>325</v>
       </c>
       <c r="B255" s="3" t="s">
         <v>364</v>
@@ -19688,7 +19688,7 @@
     </row>
     <row r="256" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>288</v>
+        <v>326</v>
       </c>
       <c r="B256" s="3" t="s">
         <v>364</v>
@@ -19759,7 +19759,7 @@
     </row>
     <row r="257" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>289</v>
+        <v>327</v>
       </c>
       <c r="B257" s="3" t="s">
         <v>364</v>
@@ -19830,7 +19830,7 @@
     </row>
     <row r="258" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>290</v>
+        <v>328</v>
       </c>
       <c r="B258" s="3" t="s">
         <v>364</v>
@@ -19901,7 +19901,7 @@
     </row>
     <row r="259" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>291</v>
+        <v>329</v>
       </c>
       <c r="B259" s="3" t="s">
         <v>364</v>
@@ -19972,7 +19972,7 @@
     </row>
     <row r="260" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>292</v>
+        <v>330</v>
       </c>
       <c r="B260" s="3" t="s">
         <v>364</v>
@@ -20043,7 +20043,7 @@
     </row>
     <row r="261" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>293</v>
+        <v>331</v>
       </c>
       <c r="B261" s="3" t="s">
         <v>364</v>
@@ -20114,7 +20114,7 @@
     </row>
     <row r="262" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>294</v>
+        <v>332</v>
       </c>
       <c r="B262" s="3" t="s">
         <v>364</v>
@@ -20185,7 +20185,7 @@
     </row>
     <row r="263" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>295</v>
+        <v>333</v>
       </c>
       <c r="B263" s="3" t="s">
         <v>364</v>
@@ -20256,7 +20256,7 @@
     </row>
     <row r="264" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>296</v>
+        <v>334</v>
       </c>
       <c r="B264" s="3" t="s">
         <v>364</v>
@@ -20327,7 +20327,7 @@
     </row>
     <row r="265" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>297</v>
+        <v>335</v>
       </c>
       <c r="B265" s="3" t="s">
         <v>364</v>
@@ -20398,7 +20398,7 @@
     </row>
     <row r="266" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>298</v>
+        <v>336</v>
       </c>
       <c r="B266" s="3" t="s">
         <v>364</v>
@@ -20469,7 +20469,7 @@
     </row>
     <row r="267" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>299</v>
+        <v>337</v>
       </c>
       <c r="B267" s="3" t="s">
         <v>364</v>
@@ -20540,7 +20540,7 @@
     </row>
     <row r="268" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>300</v>
+        <v>338</v>
       </c>
       <c r="B268" s="3" t="s">
         <v>364</v>
@@ -20611,7 +20611,7 @@
     </row>
     <row r="269" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>301</v>
+        <v>339</v>
       </c>
       <c r="B269" s="3" t="s">
         <v>364</v>
@@ -20682,7 +20682,7 @@
     </row>
     <row r="270" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>302</v>
+        <v>340</v>
       </c>
       <c r="B270" s="3" t="s">
         <v>364</v>
@@ -20753,7 +20753,7 @@
     </row>
     <row r="271" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>303</v>
+        <v>341</v>
       </c>
       <c r="B271" s="3" t="s">
         <v>364</v>
@@ -20824,7 +20824,7 @@
     </row>
     <row r="272" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>304</v>
+        <v>342</v>
       </c>
       <c r="B272" s="3" t="s">
         <v>364</v>
@@ -20895,7 +20895,7 @@
     </row>
     <row r="273" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>305</v>
+        <v>343</v>
       </c>
       <c r="B273" s="3" t="s">
         <v>364</v>
@@ -20966,7 +20966,7 @@
     </row>
     <row r="274" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>306</v>
+        <v>344</v>
       </c>
       <c r="B274" s="3" t="s">
         <v>364</v>
@@ -21037,7 +21037,7 @@
     </row>
     <row r="275" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>307</v>
+        <v>345</v>
       </c>
       <c r="B275" s="3" t="s">
         <v>364</v>
@@ -21108,7 +21108,7 @@
     </row>
     <row r="276" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>308</v>
+        <v>346</v>
       </c>
       <c r="B276" s="3" t="s">
         <v>364</v>
@@ -21179,7 +21179,7 @@
     </row>
     <row r="277" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>309</v>
+        <v>347</v>
       </c>
       <c r="B277" s="3" t="s">
         <v>364</v>
@@ -21250,7 +21250,7 @@
     </row>
     <row r="278" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>310</v>
+        <v>348</v>
       </c>
       <c r="B278" s="3" t="s">
         <v>364</v>
@@ -21321,7 +21321,7 @@
     </row>
     <row r="279" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>311</v>
+        <v>349</v>
       </c>
       <c r="B279" s="3" t="s">
         <v>364</v>
@@ -21392,7 +21392,7 @@
     </row>
     <row r="280" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>312</v>
+        <v>350</v>
       </c>
       <c r="B280" s="3" t="s">
         <v>364</v>
@@ -21422,7 +21422,7 @@
         <v>361</v>
       </c>
       <c r="L280">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M280" t="s">
         <v>31</v>
@@ -21463,7 +21463,7 @@
     </row>
     <row r="281" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>313</v>
+        <v>351</v>
       </c>
       <c r="B281" s="3" t="s">
         <v>364</v>
@@ -21493,7 +21493,7 @@
         <v>361</v>
       </c>
       <c r="L281">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="M281" t="s">
         <v>31</v>
@@ -21534,7 +21534,7 @@
     </row>
     <row r="282" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>314</v>
+        <v>352</v>
       </c>
       <c r="B282" s="3" t="s">
         <v>364</v>
@@ -21605,7 +21605,7 @@
     </row>
     <row r="283" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>315</v>
+        <v>353</v>
       </c>
       <c r="B283" s="3" t="s">
         <v>364</v>
@@ -21676,7 +21676,7 @@
     </row>
     <row r="284" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>316</v>
+        <v>354</v>
       </c>
       <c r="B284" s="3" t="s">
         <v>364</v>
@@ -21747,7 +21747,7 @@
     </row>
     <row r="285" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>317</v>
+        <v>355</v>
       </c>
       <c r="B285" s="3" t="s">
         <v>364</v>
@@ -21818,7 +21818,7 @@
     </row>
     <row r="286" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>318</v>
+        <v>356</v>
       </c>
       <c r="B286" s="3" t="s">
         <v>364</v>
@@ -21889,7 +21889,7 @@
     </row>
     <row r="287" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>319</v>
+        <v>357</v>
       </c>
       <c r="B287" s="3" t="s">
         <v>364</v>
@@ -21960,7 +21960,7 @@
     </row>
     <row r="288" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>320</v>
+        <v>358</v>
       </c>
       <c r="B288" s="3" t="s">
         <v>364</v>
@@ -22031,7 +22031,7 @@
     </row>
     <row r="289" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>321</v>
+        <v>34</v>
       </c>
       <c r="B289" s="3" t="s">
         <v>364</v>
@@ -22102,7 +22102,7 @@
     </row>
     <row r="290" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>322</v>
+        <v>35</v>
       </c>
       <c r="B290" s="3" t="s">
         <v>364</v>
@@ -22173,7 +22173,7 @@
     </row>
     <row r="291" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>323</v>
+        <v>36</v>
       </c>
       <c r="B291" s="3" t="s">
         <v>364</v>
@@ -22244,7 +22244,7 @@
     </row>
     <row r="292" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>324</v>
+        <v>37</v>
       </c>
       <c r="B292" s="3" t="s">
         <v>364</v>
@@ -22315,7 +22315,7 @@
     </row>
     <row r="293" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>325</v>
+        <v>38</v>
       </c>
       <c r="B293" s="3" t="s">
         <v>364</v>
@@ -22386,7 +22386,7 @@
     </row>
     <row r="294" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>326</v>
+        <v>39</v>
       </c>
       <c r="B294" s="3" t="s">
         <v>364</v>
@@ -22457,7 +22457,7 @@
     </row>
     <row r="295" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>327</v>
+        <v>40</v>
       </c>
       <c r="B295" s="3" t="s">
         <v>364</v>
@@ -22528,7 +22528,7 @@
     </row>
     <row r="296" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>328</v>
+        <v>41</v>
       </c>
       <c r="B296" s="3" t="s">
         <v>364</v>
@@ -22599,7 +22599,7 @@
     </row>
     <row r="297" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>329</v>
+        <v>42</v>
       </c>
       <c r="B297" s="3" t="s">
         <v>364</v>
@@ -22670,7 +22670,7 @@
     </row>
     <row r="298" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>330</v>
+        <v>43</v>
       </c>
       <c r="B298" s="3" t="s">
         <v>364</v>
@@ -22741,7 +22741,7 @@
     </row>
     <row r="299" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>331</v>
+        <v>44</v>
       </c>
       <c r="B299" s="3" t="s">
         <v>364</v>
@@ -22812,7 +22812,7 @@
     </row>
     <row r="300" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>332</v>
+        <v>45</v>
       </c>
       <c r="B300" s="3" t="s">
         <v>364</v>
@@ -22883,7 +22883,7 @@
     </row>
     <row r="301" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>333</v>
+        <v>46</v>
       </c>
       <c r="B301" s="3" t="s">
         <v>364</v>
@@ -22954,7 +22954,7 @@
     </row>
     <row r="302" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>334</v>
+        <v>47</v>
       </c>
       <c r="B302" s="3" t="s">
         <v>364</v>
@@ -23025,7 +23025,7 @@
     </row>
     <row r="303" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>335</v>
+        <v>48</v>
       </c>
       <c r="B303" s="3" t="s">
         <v>364</v>
@@ -23096,7 +23096,7 @@
     </row>
     <row r="304" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>336</v>
+        <v>49</v>
       </c>
       <c r="B304" s="3" t="s">
         <v>364</v>
@@ -23167,7 +23167,7 @@
     </row>
     <row r="305" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>337</v>
+        <v>50</v>
       </c>
       <c r="B305" s="3" t="s">
         <v>364</v>
@@ -23238,7 +23238,7 @@
     </row>
     <row r="306" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>338</v>
+        <v>51</v>
       </c>
       <c r="B306" s="3" t="s">
         <v>364</v>
@@ -23309,7 +23309,7 @@
     </row>
     <row r="307" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>339</v>
+        <v>52</v>
       </c>
       <c r="B307" s="3" t="s">
         <v>364</v>
@@ -23380,7 +23380,7 @@
     </row>
     <row r="308" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>340</v>
+        <v>53</v>
       </c>
       <c r="B308" s="3" t="s">
         <v>364</v>
@@ -23451,7 +23451,7 @@
     </row>
     <row r="309" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>341</v>
+        <v>54</v>
       </c>
       <c r="B309" s="3" t="s">
         <v>364</v>
@@ -23522,7 +23522,7 @@
     </row>
     <row r="310" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>342</v>
+        <v>55</v>
       </c>
       <c r="B310" s="3" t="s">
         <v>364</v>
@@ -23593,7 +23593,7 @@
     </row>
     <row r="311" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>343</v>
+        <v>56</v>
       </c>
       <c r="B311" s="3" t="s">
         <v>364</v>
@@ -23664,7 +23664,7 @@
     </row>
     <row r="312" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>344</v>
+        <v>57</v>
       </c>
       <c r="B312" s="3" t="s">
         <v>364</v>
@@ -23735,7 +23735,7 @@
     </row>
     <row r="313" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>345</v>
+        <v>58</v>
       </c>
       <c r="B313" s="3" t="s">
         <v>364</v>
@@ -23806,7 +23806,7 @@
     </row>
     <row r="314" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>346</v>
+        <v>59</v>
       </c>
       <c r="B314" s="3" t="s">
         <v>364</v>
@@ -23877,7 +23877,7 @@
     </row>
     <row r="315" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>347</v>
+        <v>60</v>
       </c>
       <c r="B315" s="3" t="s">
         <v>364</v>
@@ -23948,7 +23948,7 @@
     </row>
     <row r="316" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>348</v>
+        <v>61</v>
       </c>
       <c r="B316" s="3" t="s">
         <v>364</v>
@@ -24019,7 +24019,7 @@
     </row>
     <row r="317" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>349</v>
+        <v>62</v>
       </c>
       <c r="B317" s="3" t="s">
         <v>364</v>
@@ -24090,7 +24090,7 @@
     </row>
     <row r="318" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>350</v>
+        <v>63</v>
       </c>
       <c r="B318" s="3" t="s">
         <v>364</v>
@@ -24120,7 +24120,7 @@
         <v>361</v>
       </c>
       <c r="L318">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M318" t="s">
         <v>31</v>
@@ -24161,7 +24161,7 @@
     </row>
     <row r="319" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>351</v>
+        <v>64</v>
       </c>
       <c r="B319" s="3" t="s">
         <v>364</v>
@@ -24191,7 +24191,7 @@
         <v>361</v>
       </c>
       <c r="L319">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="M319" t="s">
         <v>31</v>
@@ -24232,7 +24232,7 @@
     </row>
     <row r="320" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>352</v>
+        <v>65</v>
       </c>
       <c r="B320" s="3" t="s">
         <v>364</v>
@@ -24303,7 +24303,7 @@
     </row>
     <row r="321" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>353</v>
+        <v>66</v>
       </c>
       <c r="B321" s="3" t="s">
         <v>364</v>
@@ -24374,7 +24374,7 @@
     </row>
     <row r="322" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>354</v>
+        <v>67</v>
       </c>
       <c r="B322" s="3" t="s">
         <v>364</v>
@@ -24445,7 +24445,7 @@
     </row>
     <row r="323" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>355</v>
+        <v>68</v>
       </c>
       <c r="B323" s="3" t="s">
         <v>364</v>
@@ -24516,7 +24516,7 @@
     </row>
     <row r="324" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>356</v>
+        <v>69</v>
       </c>
       <c r="B324" s="3" t="s">
         <v>364</v>
@@ -24587,7 +24587,7 @@
     </row>
     <row r="325" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>357</v>
+        <v>70</v>
       </c>
       <c r="B325" s="3" t="s">
         <v>364</v>
@@ -24658,7 +24658,7 @@
     </row>
     <row r="326" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>358</v>
+        <v>71</v>
       </c>
       <c r="B326" s="3" t="s">
         <v>364</v>
@@ -24728,11 +24728,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB326" xr:uid="{1CEE0A21-2F00-CE4A-80DF-F7E5013BA5D9}"/>
+  <autoFilter ref="A1:AB288" xr:uid="{1CEE0A21-2F00-CE4A-80DF-F7E5013BA5D9}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{C3618B20-945E-DB4F-90FC-3A6B7E48AEC3}"/>
-    <hyperlink ref="B3:B326" r:id="rId2" display="sdumas@premiumparking.com" xr:uid="{83FF5FA2-97C8-4868-AEFC-B622F077C803}"/>
+    <hyperlink ref="B289" r:id="rId1" xr:uid="{C3618B20-945E-DB4F-90FC-3A6B7E48AEC3}"/>
+    <hyperlink ref="B2:B288" r:id="rId2" display="sdumas@premiumparking.com" xr:uid="{83FF5FA2-97C8-4868-AEFC-B622F077C803}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -25002,11 +25002,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489367A9-E8D5-45F0-91B8-31D59E518767}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="55.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>